<commit_message>
Change in excel and added tags of OPR344
</commit_message>
<xml_diff>
--- a/TestData/OPR344_ExportManifest_TestData.xlsx
+++ b/TestData/OPR344_ExportManifest_TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-ssaha1\Desktop\ICargo KT\Xunit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Automation 2025\Xunit Sprint 7\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F9FB1B-8698-490B-BC29-75551A01EA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46E08D8-85F1-4645-84D9-93F261543FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="16" activeTab="18" xr2:uid="{4A2F2A72-D862-47A0-B5E4-CC538090D2B0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4A2F2A72-D862-47A0-B5E4-CC538090D2B0}"/>
   </bookViews>
   <sheets>
     <sheet name="OPR344_EXP_00001" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="66">
   <si>
     <t>AgentCode</t>
   </si>
@@ -260,10 +260,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -626,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3405C8-064D-439D-892A-250B297B720F}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -638,7 +644,7 @@
     <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
@@ -747,7 +753,558 @@
         <v>25</v>
       </c>
     </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>10763</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <v>13</v>
+      </c>
+      <c r="L3">
+        <v>775</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>10763</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <v>2199</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>360</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>10763</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5">
+        <v>13</v>
+      </c>
+      <c r="L5">
+        <v>775</v>
+      </c>
+      <c r="M5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>10763</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6">
+        <v>13</v>
+      </c>
+      <c r="L6">
+        <v>775</v>
+      </c>
+      <c r="M6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>10763</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <v>2199</v>
+      </c>
+      <c r="I7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>360</v>
+      </c>
+      <c r="M7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>10763</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8">
+        <v>13</v>
+      </c>
+      <c r="L8">
+        <v>775</v>
+      </c>
+      <c r="M8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>10763</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9">
+        <v>13</v>
+      </c>
+      <c r="L9">
+        <v>775</v>
+      </c>
+      <c r="M9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>10763</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10">
+        <v>2199</v>
+      </c>
+      <c r="I10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>360</v>
+      </c>
+      <c r="M10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>10763</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11">
+        <v>13</v>
+      </c>
+      <c r="L11">
+        <v>775</v>
+      </c>
+      <c r="M11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>10763</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12">
+        <v>13</v>
+      </c>
+      <c r="L12">
+        <v>775</v>
+      </c>
+      <c r="M12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>10763</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13">
+        <v>2199</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13">
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <v>360</v>
+      </c>
+      <c r="M13" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2021,7 +2578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A475D373-CE6A-4A53-8458-E7291611DAD3}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change in maintain booking page select flight function
</commit_message>
<xml_diff>
--- a/TestData/OPR344_ExportManifest_TestData.xlsx
+++ b/TestData/OPR344_ExportManifest_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-asaha\Automation 2025\Xunit Sprint 7\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-vkaushal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46E08D8-85F1-4645-84D9-93F261543FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C478B5-174E-42DC-AB8C-321A4383CA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4A2F2A72-D862-47A0-B5E4-CC538090D2B0}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="21570" windowHeight="12870" firstSheet="3" activeTab="6" xr2:uid="{4A2F2A72-D862-47A0-B5E4-CC538090D2B0}"/>
   </bookViews>
   <sheets>
     <sheet name="OPR344_EXP_00001" sheetId="1" r:id="rId1"/>
@@ -19,21 +19,22 @@
     <sheet name="OPR344_EXP_00004" sheetId="4" r:id="rId4"/>
     <sheet name="OPR344_EXP_00005" sheetId="5" r:id="rId5"/>
     <sheet name="OPR344_EXP_00006" sheetId="6" r:id="rId6"/>
-    <sheet name="OPR344_EXP_00010" sheetId="7" r:id="rId7"/>
-    <sheet name="OPR344_EXP_00011" sheetId="8" r:id="rId8"/>
-    <sheet name="OPR344_EXP_00012" sheetId="9" r:id="rId9"/>
-    <sheet name="OPR344_EXP_00013" sheetId="10" r:id="rId10"/>
-    <sheet name="OPR344_EXP_00014" sheetId="11" r:id="rId11"/>
-    <sheet name="OPR344_EXP_00015" sheetId="12" r:id="rId12"/>
-    <sheet name="OPR344_EXP_00017" sheetId="13" r:id="rId13"/>
-    <sheet name="OPR344_EXP_00018" sheetId="14" r:id="rId14"/>
-    <sheet name="OPR344_EXP_00020" sheetId="15" r:id="rId15"/>
-    <sheet name="OPR344_EXP_00021" sheetId="16" r:id="rId16"/>
-    <sheet name="OPR344_EXP_00022" sheetId="17" r:id="rId17"/>
-    <sheet name="OPR344_EXP_00025" sheetId="18" r:id="rId18"/>
-    <sheet name="OPR344_EXP_00026" sheetId="19" r:id="rId19"/>
-    <sheet name="OPR344_EXP_00027" sheetId="20" r:id="rId20"/>
-    <sheet name="OPR344_EXP_00028" sheetId="21" r:id="rId21"/>
+    <sheet name="OPR344_EXP_00008" sheetId="22" r:id="rId7"/>
+    <sheet name="OPR344_EXP_00010" sheetId="7" r:id="rId8"/>
+    <sheet name="OPR344_EXP_00011" sheetId="8" r:id="rId9"/>
+    <sheet name="OPR344_EXP_00012" sheetId="9" r:id="rId10"/>
+    <sheet name="OPR344_EXP_00013" sheetId="10" r:id="rId11"/>
+    <sheet name="OPR344_EXP_00014" sheetId="11" r:id="rId12"/>
+    <sheet name="OPR344_EXP_00015" sheetId="12" r:id="rId13"/>
+    <sheet name="OPR344_EXP_00017" sheetId="13" r:id="rId14"/>
+    <sheet name="OPR344_EXP_00018" sheetId="14" r:id="rId15"/>
+    <sheet name="OPR344_EXP_00020" sheetId="15" r:id="rId16"/>
+    <sheet name="OPR344_EXP_00021" sheetId="16" r:id="rId17"/>
+    <sheet name="OPR344_EXP_00022" sheetId="17" r:id="rId18"/>
+    <sheet name="OPR344_EXP_00025" sheetId="18" r:id="rId19"/>
+    <sheet name="OPR344_EXP_00026" sheetId="19" r:id="rId20"/>
+    <sheet name="OPR344_EXP_00027" sheetId="20" r:id="rId21"/>
+    <sheet name="OPR344_EXP_00028" sheetId="21" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="66">
   <si>
     <t>AgentCode</t>
   </si>
@@ -260,16 +261,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -632,28 +627,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE3405C8-064D-439D-892A-250B297B720F}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +698,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -753,586 +748,36 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
-        <v>10763</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3">
-        <v>13</v>
-      </c>
-      <c r="L3">
-        <v>775</v>
-      </c>
-      <c r="M3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>10763</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4">
-        <v>2199</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4">
-        <v>8</v>
-      </c>
-      <c r="L4">
-        <v>360</v>
-      </c>
-      <c r="M4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5">
-        <v>10763</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5">
-        <v>13</v>
-      </c>
-      <c r="L5">
-        <v>775</v>
-      </c>
-      <c r="M5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>10763</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6">
-        <v>13</v>
-      </c>
-      <c r="L6">
-        <v>775</v>
-      </c>
-      <c r="M6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>10763</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7">
-        <v>2199</v>
-      </c>
-      <c r="I7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7">
-        <v>8</v>
-      </c>
-      <c r="L7">
-        <v>360</v>
-      </c>
-      <c r="M7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>10763</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8">
-        <v>13</v>
-      </c>
-      <c r="L8">
-        <v>775</v>
-      </c>
-      <c r="M8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8" t="s">
-        <v>24</v>
-      </c>
-      <c r="P8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>10763</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9">
-        <v>13</v>
-      </c>
-      <c r="L9">
-        <v>775</v>
-      </c>
-      <c r="M9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" t="s">
-        <v>21</v>
-      </c>
-      <c r="O9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>10763</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10">
-        <v>2199</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10">
-        <v>8</v>
-      </c>
-      <c r="L10">
-        <v>360</v>
-      </c>
-      <c r="M10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>10763</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11">
-        <v>13</v>
-      </c>
-      <c r="L11">
-        <v>775</v>
-      </c>
-      <c r="M11" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" t="s">
-        <v>21</v>
-      </c>
-      <c r="O11" t="s">
-        <v>24</v>
-      </c>
-      <c r="P11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <v>10763</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12">
-        <v>13</v>
-      </c>
-      <c r="L12">
-        <v>775</v>
-      </c>
-      <c r="M12" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" t="s">
-        <v>21</v>
-      </c>
-      <c r="O12" t="s">
-        <v>24</v>
-      </c>
-      <c r="P12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <v>10763</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13">
-        <v>2199</v>
-      </c>
-      <c r="I13" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13">
-        <v>8</v>
-      </c>
-      <c r="L13">
-        <v>360</v>
-      </c>
-      <c r="M13" t="s">
-        <v>23</v>
-      </c>
-      <c r="N13" t="s">
-        <v>21</v>
-      </c>
-      <c r="O13" t="s">
-        <v>24</v>
-      </c>
-      <c r="P13" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8DFE2F-9ACE-4F06-9DF8-4475B0A3C877}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077EDD78-85E4-4FE1-B4AE-C737151368FA}">
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1376,13 +821,16 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -1393,13 +841,13 @@
         <v>11377</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -1414,10 +862,10 @@
         <v>21</v>
       </c>
       <c r="K2">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="L2">
-        <v>198</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s">
         <v>23</v>
@@ -1425,42 +873,99 @@
       <c r="N2" t="s">
         <v>21</v>
       </c>
-      <c r="O2" t="s">
-        <v>25</v>
+      <c r="O2">
+        <v>155</v>
       </c>
       <c r="P2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>59</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3">
+        <v>155</v>
+      </c>
+      <c r="P3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7043FCA6-2FB3-4A38-9F0C-7E211FC123E2}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C8DFE2F-9ACE-4F06-9DF8-4475B0A3C877}">
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1510,7 +1015,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -1527,7 +1032,7 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -1542,10 +1047,10 @@
         <v>21</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="L2">
-        <v>59</v>
+        <v>198</v>
       </c>
       <c r="M2" t="s">
         <v>23</v>
@@ -1557,6 +1062,56 @@
         <v>25</v>
       </c>
       <c r="P2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <v>14</v>
+      </c>
+      <c r="L3">
+        <v>198</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1566,30 +1121,29 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8718DD54-2741-4A68-8950-E5F34692E75E}">
-  <dimension ref="A1:Q2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7043FCA6-2FB3-4A38-9F0C-7E211FC123E2}">
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1636,13 +1190,10 @@
         <v>15</v>
       </c>
       <c r="P1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -1659,14 +1210,13 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="str">
-        <f>"0"&amp;316</f>
-        <v>0316</v>
+      <c r="H2" t="s">
+        <v>22</v>
       </c>
       <c r="I2" t="s">
         <v>21</v>
@@ -1689,10 +1239,57 @@
       <c r="O2" t="s">
         <v>25</v>
       </c>
-      <c r="P2">
-        <v>34</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="P2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>59</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1702,6 +1299,196 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8718DD54-2741-4A68-8950-E5F34692E75E}">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="str">
+        <f>"0"&amp;316</f>
+        <v>0316</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>59</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="str">
+        <f>"0"&amp;316</f>
+        <v>0316</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>59</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3">
+        <v>26</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04EA279-8D72-42BF-A62F-F24DC5DD6715}">
   <dimension ref="A1:V2"/>
   <sheetViews>
@@ -1709,28 +1496,28 @@
       <selection activeCell="J1" sqref="J1:V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1798,7 +1585,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -1871,7 +1658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1970537-3C0D-4B1C-B282-578DB1BA6295}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -1879,23 +1666,23 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1948,7 +1735,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2007,7 +1794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858D018B-7C88-4952-80F9-648942F3CC51}">
   <dimension ref="A1:W2"/>
   <sheetViews>
@@ -2015,27 +1802,27 @@
       <selection sqref="A1:U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2106,7 +1893,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -2182,7 +1969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DB051C-C034-4D73-97FA-BEBE8E9EA08C}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -2190,22 +1977,22 @@
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2255,7 +2042,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -2310,7 +2097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64935B7F-8999-44FA-A06A-05EB468DD0E7}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -2318,22 +2105,22 @@
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2383,7 +2170,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -2431,142 +2218,6 @@
       </c>
       <c r="P2" t="s">
         <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64195E5B-8F95-4294-9D13-F7FF6F145626}">
-  <dimension ref="A1:Q2"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.08984375" customWidth="1"/>
-    <col min="17" max="18" width="9.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2">
-        <v>11377</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2">
-        <v>60</v>
-      </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2">
-        <v>65</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2575,35 +2226,36 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A475D373-CE6A-4A53-8458-E7291611DAD3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64195E5B-8F95-4294-9D13-F7FF6F145626}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" customWidth="1"/>
+    <col min="17" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2651,12 +2303,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>11377</v>
-      </c>
-      <c r="B2">
-        <v>11377</v>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
       </c>
       <c r="C2">
         <v>11377</v>
@@ -2695,7 +2347,7 @@
         <v>21</v>
       </c>
       <c r="O2">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="P2" t="s">
         <v>24</v>
@@ -2717,23 +2369,23 @@
       <selection sqref="A1:Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2786,7 +2438,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -2845,6 +2497,141 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A475D373-CE6A-4A53-8458-E7291611DAD3}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11377</v>
+      </c>
+      <c r="B2">
+        <v>11377</v>
+      </c>
+      <c r="C2">
+        <v>11377</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>60</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2">
+        <v>173</v>
+      </c>
+      <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4857B88B-AC0A-4EEA-8393-5AE17685CCF6}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
@@ -2852,24 +2639,24 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.1796875" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.7265625" customWidth="1"/>
-    <col min="17" max="17" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2922,7 +2709,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>16956</v>
       </c>
@@ -2975,7 +2762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>16956</v>
       </c>
@@ -3033,7 +2820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9ECBA3E-2EB5-4280-97C6-AE6B82AA22B5}">
   <dimension ref="A1:V2"/>
   <sheetViews>
@@ -3041,28 +2828,28 @@
       <selection sqref="A1:V1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3130,7 +2917,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -3211,22 +2998,22 @@
       <selection sqref="A1:P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3276,7 +3063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -3326,7 +3113,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -3376,7 +3163,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>11377</v>
       </c>
@@ -3435,27 +3222,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD3E9EF-A87F-4EE0-BD3F-AEACF3F3762C}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3508,7 +3295,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -3561,7 +3348,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -3627,23 +3414,23 @@
       <selection sqref="A1:Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3696,7 +3483,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -3759,25 +3546,25 @@
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3833,7 +3620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -3889,7 +3676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -3945,7 +3732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -4007,29 +3794,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55838455-B793-459B-B87F-42BC45E9C52F}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7EB7B2-8380-49FF-997B-C789FAAD50D3}">
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4079,7 +3853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -4090,10 +3864,10 @@
         <v>11377</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -4101,8 +3875,8 @@
       <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
-        <v>22</v>
+      <c r="H2" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="I2" t="s">
         <v>21</v>
@@ -4114,7 +3888,7 @@
         <v>2</v>
       </c>
       <c r="L2">
-        <v>59</v>
+        <v>234</v>
       </c>
       <c r="M2" t="s">
         <v>23</v>
@@ -4126,6 +3900,56 @@
         <v>25</v>
       </c>
       <c r="P2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3">
+        <v>2199</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>189</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4135,29 +3959,29 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B4E1ED3-0D31-416C-90F1-02848B1B322D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55838455-B793-459B-B87F-42BC45E9C52F}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4207,7 +4031,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -4218,13 +4042,13 @@
         <v>11377</v>
       </c>
       <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
-        <v>58</v>
-      </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -4257,7 +4081,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11377</v>
       </c>
@@ -4268,10 +4092,10 @@
         <v>11377</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>58</v>
       </c>
       <c r="F3" t="s">
         <v>39</v>
@@ -4279,8 +4103,8 @@
       <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="H3">
-        <v>2199</v>
+      <c r="H3" t="s">
+        <v>22</v>
       </c>
       <c r="I3" t="s">
         <v>21</v>
@@ -4289,10 +4113,10 @@
         <v>21</v>
       </c>
       <c r="K3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L3">
-        <v>287</v>
+        <v>59</v>
       </c>
       <c r="M3" t="s">
         <v>23</v>
@@ -4313,30 +4137,29 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077EDD78-85E4-4FE1-B4AE-C737151368FA}">
-  <dimension ref="A1:Q2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B4E1ED3-0D31-416C-90F1-02848B1B322D}">
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4380,16 +4203,13 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11377</v>
       </c>
@@ -4406,7 +4226,7 @@
         <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -4432,18 +4252,64 @@
       <c r="N2" t="s">
         <v>21</v>
       </c>
-      <c r="O2">
-        <v>155</v>
+      <c r="O2" t="s">
+        <v>25</v>
       </c>
       <c r="P2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11377</v>
+      </c>
+      <c r="B3">
+        <v>11377</v>
+      </c>
+      <c r="C3">
+        <v>11377</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3">
+        <v>2199</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>287</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P3" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>